<commit_message>
Commiting the acc to legal agreement flow
</commit_message>
<xml_diff>
--- a/Omnitracs/src/test/resources/Excel/TestCases.xlsx
+++ b/Omnitracs/src/test/resources/Excel/TestCases.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Selenium\Workspace\Omnitracs\src\test\resources\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rselvanambi\eclipse-workspace\Omnitracs\src\test\resources\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32994FBB-35F9-4011-AE63-6E0C097946C2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{683E49A6-4AF5-4493-98E0-0D34BAC84C6B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3680" yWindow="460" windowWidth="14980" windowHeight="9240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TestCases" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>TestCaseName</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t>Yes</t>
+  </si>
+  <si>
+    <t>AcctoLegalAgreement</t>
   </si>
 </sst>
 </file>
@@ -362,10 +365,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -479,11 +482,22 @@
         <v>21</v>
       </c>
       <c r="C9" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>23</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C10" s="2"/>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C11" s="2"/>
+    </row>
+    <row r="12" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C12" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>